<commit_message>
Committed the changes related to batch run
</commit_message>
<xml_diff>
--- a/input/Mendix_TestPlan.xlsx
+++ b/input/Mendix_TestPlan.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FinalBatchrun\Mendix\Mendix\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Branching\Mendix_BatchRun\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D4F80A-0051-42A4-B0C8-758B73E65E87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B5BE9C-EACD-49D1-9BF1-68754647CFF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{14E9EC64-EF31-48E0-B023-FAA0F7238E1E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="113">
   <si>
     <t>35Create_Material_SaveAsDraft_JDE.xml</t>
   </si>
@@ -365,13 +365,17 @@
     <t>abc</t>
   </si>
   <si>
-    <t>512374</t>
+    <t>505326</t>
+  </si>
+  <si>
+    <t>1427470</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -749,20 +753,20 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="72" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.85546875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="97.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="9.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="72.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -849,7 +853,7 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>111</v>

</xml_diff>